<commit_message>
final standard tweaks include update spreadsheet
</commit_message>
<xml_diff>
--- a/app/assets/standard-points-guidance-v01-dec-2022.xlsx
+++ b/app/assets/standard-points-guidance-v01-dec-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andyjones/Source/apply-service-standard-in-dfe/source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kerrylyons/Documents/Source/dfe-standards-manual-prototype/app/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71A0D9D9-43AC-724D-8008-DE92320BDDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEEBC1F-F115-1047-B3FF-F0A01FBF46D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39380" yWindow="1740" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="267">
   <si>
     <t>Apply the Service Standard in DfE</t>
   </si>
@@ -2258,6 +2258,9 @@
       <t xml:space="preserve"> has been started, where necessary. If you do not have access to the DfE intranet, ask a civil servant to get the information for you</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">evidence that the security controls implemented are compliant with department standards </t>
+  </si>
 </sst>
 </file>
 
@@ -2266,7 +2269,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2368,6 +2371,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2401,7 +2411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2438,6 +2448,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2658,7 +2669,7 @@
   </sheetPr>
   <dimension ref="B3:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -2813,13 +2824,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1008"/>
+  <dimension ref="A1:AA1009"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D156" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13"/>
@@ -9637,7 +9648,7 @@
       <c r="Z184" s="9"/>
       <c r="AA184" s="9"/>
     </row>
-    <row r="185" spans="1:27" ht="14">
+    <row r="185" spans="1:27">
       <c r="A185" s="9">
         <v>9</v>
       </c>
@@ -9647,8 +9658,8 @@
       <c r="C185" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D185" s="10" t="s">
-        <v>213</v>
+      <c r="D185" s="18" t="s">
+        <v>266</v>
       </c>
       <c r="E185" s="9"/>
       <c r="F185" s="9"/>
@@ -9685,7 +9696,7 @@
         <v>51</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E186" s="9"/>
       <c r="F186" s="9"/>
@@ -9722,7 +9733,7 @@
         <v>51</v>
       </c>
       <c r="D187" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E187" s="9"/>
       <c r="F187" s="9"/>
@@ -9748,7 +9759,7 @@
       <c r="Z187" s="9"/>
       <c r="AA187" s="9"/>
     </row>
-    <row r="188" spans="1:27">
+    <row r="188" spans="1:27" ht="14">
       <c r="A188" s="9">
         <v>9</v>
       </c>
@@ -9758,8 +9769,8 @@
       <c r="C188" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D188" s="14" t="s">
-        <v>216</v>
+      <c r="D188" s="10" t="s">
+        <v>215</v>
       </c>
       <c r="E188" s="9"/>
       <c r="F188" s="9"/>
@@ -9785,18 +9796,18 @@
       <c r="Z188" s="9"/>
       <c r="AA188" s="9"/>
     </row>
-    <row r="189" spans="1:27" ht="14">
+    <row r="189" spans="1:27">
       <c r="A189" s="9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D189" s="10" t="s">
-        <v>218</v>
+        <v>51</v>
+      </c>
+      <c r="D189" s="14" t="s">
+        <v>216</v>
       </c>
       <c r="E189" s="9"/>
       <c r="F189" s="9"/>
@@ -9833,7 +9844,7 @@
         <v>34</v>
       </c>
       <c r="D190" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E190" s="9"/>
       <c r="F190" s="9"/>
@@ -9869,8 +9880,8 @@
       <c r="C191" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D191" s="11" t="s">
-        <v>220</v>
+      <c r="D191" s="10" t="s">
+        <v>219</v>
       </c>
       <c r="E191" s="9"/>
       <c r="F191" s="9"/>
@@ -9906,8 +9917,8 @@
       <c r="C192" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D192" s="10" t="s">
-        <v>221</v>
+      <c r="D192" s="11" t="s">
+        <v>220</v>
       </c>
       <c r="E192" s="9"/>
       <c r="F192" s="9"/>
@@ -9944,7 +9955,7 @@
         <v>34</v>
       </c>
       <c r="D193" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E193" s="9"/>
       <c r="F193" s="9"/>
@@ -9981,7 +9992,7 @@
         <v>34</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E194" s="9"/>
       <c r="F194" s="9"/>
@@ -10018,7 +10029,7 @@
         <v>34</v>
       </c>
       <c r="D195" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E195" s="9"/>
       <c r="F195" s="9"/>
@@ -10052,10 +10063,10 @@
         <v>217</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D196" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E196" s="9"/>
       <c r="F196" s="9"/>
@@ -10092,7 +10103,7 @@
         <v>51</v>
       </c>
       <c r="D197" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E197" s="9"/>
       <c r="F197" s="9"/>
@@ -10129,7 +10140,7 @@
         <v>51</v>
       </c>
       <c r="D198" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E198" s="9"/>
       <c r="F198" s="9"/>
@@ -10166,7 +10177,7 @@
         <v>51</v>
       </c>
       <c r="D199" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E199" s="9"/>
       <c r="F199" s="9"/>
@@ -10203,7 +10214,7 @@
         <v>51</v>
       </c>
       <c r="D200" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E200" s="9"/>
       <c r="F200" s="9"/>
@@ -10240,7 +10251,7 @@
         <v>51</v>
       </c>
       <c r="D201" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E201" s="9"/>
       <c r="F201" s="9"/>
@@ -10276,8 +10287,8 @@
       <c r="C202" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D202" s="11" t="s">
-        <v>231</v>
+      <c r="D202" s="10" t="s">
+        <v>230</v>
       </c>
       <c r="E202" s="9"/>
       <c r="F202" s="9"/>
@@ -10313,8 +10324,8 @@
       <c r="C203" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D203" s="10" t="s">
-        <v>232</v>
+      <c r="D203" s="11" t="s">
+        <v>231</v>
       </c>
       <c r="E203" s="9"/>
       <c r="F203" s="9"/>
@@ -10342,16 +10353,16 @@
     </row>
     <row r="204" spans="1:27" ht="14">
       <c r="A204" s="9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>172</v>
+        <v>51</v>
       </c>
       <c r="D204" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E204" s="9"/>
       <c r="F204" s="9"/>
@@ -10387,8 +10398,8 @@
       <c r="C205" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D205" s="11" t="s">
-        <v>235</v>
+      <c r="D205" s="10" t="s">
+        <v>234</v>
       </c>
       <c r="E205" s="9"/>
       <c r="F205" s="9"/>
@@ -10424,8 +10435,8 @@
       <c r="C206" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D206" s="10" t="s">
-        <v>236</v>
+      <c r="D206" s="11" t="s">
+        <v>235</v>
       </c>
       <c r="E206" s="9"/>
       <c r="F206" s="9"/>
@@ -10461,8 +10472,8 @@
       <c r="C207" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D207" s="11" t="s">
-        <v>237</v>
+      <c r="D207" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="E207" s="9"/>
       <c r="F207" s="9"/>
@@ -10498,8 +10509,8 @@
       <c r="C208" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D208" s="10" t="s">
-        <v>238</v>
+      <c r="D208" s="11" t="s">
+        <v>237</v>
       </c>
       <c r="E208" s="9"/>
       <c r="F208" s="9"/>
@@ -10535,8 +10546,8 @@
       <c r="C209" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D209" s="11" t="s">
-        <v>239</v>
+      <c r="D209" s="10" t="s">
+        <v>238</v>
       </c>
       <c r="E209" s="9"/>
       <c r="F209" s="9"/>
@@ -10572,8 +10583,8 @@
       <c r="C210" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D210" s="10" t="s">
-        <v>240</v>
+      <c r="D210" s="11" t="s">
+        <v>239</v>
       </c>
       <c r="E210" s="9"/>
       <c r="F210" s="9"/>
@@ -10609,8 +10620,8 @@
       <c r="C211" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D211" s="11" t="s">
-        <v>241</v>
+      <c r="D211" s="10" t="s">
+        <v>240</v>
       </c>
       <c r="E211" s="9"/>
       <c r="F211" s="9"/>
@@ -10646,8 +10657,8 @@
       <c r="C212" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D212" s="10" t="s">
-        <v>242</v>
+      <c r="D212" s="11" t="s">
+        <v>241</v>
       </c>
       <c r="E212" s="9"/>
       <c r="F212" s="9"/>
@@ -10683,8 +10694,8 @@
       <c r="C213" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D213" s="11" t="s">
-        <v>243</v>
+      <c r="D213" s="10" t="s">
+        <v>242</v>
       </c>
       <c r="E213" s="9"/>
       <c r="F213" s="9"/>
@@ -10712,16 +10723,16 @@
     </row>
     <row r="214" spans="1:27" ht="14">
       <c r="A214" s="9">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="C214" s="9" t="s">
         <v>172</v>
       </c>
       <c r="D214" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E214" s="9"/>
       <c r="F214" s="9"/>
@@ -10749,16 +10760,16 @@
     </row>
     <row r="215" spans="1:27" ht="14">
       <c r="A215" s="9">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C215" s="9" t="s">
         <v>172</v>
       </c>
       <c r="D215" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E215" s="9"/>
       <c r="F215" s="9"/>
@@ -10795,7 +10806,7 @@
         <v>172</v>
       </c>
       <c r="D216" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E216" s="9"/>
       <c r="F216" s="9"/>
@@ -10832,7 +10843,7 @@
         <v>172</v>
       </c>
       <c r="D217" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E217" s="9"/>
       <c r="F217" s="9"/>
@@ -10869,7 +10880,7 @@
         <v>172</v>
       </c>
       <c r="D218" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E218" s="9"/>
       <c r="F218" s="9"/>
@@ -10906,7 +10917,7 @@
         <v>172</v>
       </c>
       <c r="D219" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E219" s="9"/>
       <c r="F219" s="9"/>
@@ -10943,7 +10954,7 @@
         <v>172</v>
       </c>
       <c r="D220" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E220" s="9"/>
       <c r="F220" s="9"/>
@@ -10971,16 +10982,16 @@
     </row>
     <row r="221" spans="1:27" ht="14">
       <c r="A221" s="9">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C221" s="9" t="s">
         <v>172</v>
       </c>
       <c r="D221" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E221" s="9"/>
       <c r="F221" s="9"/>
@@ -11006,7 +11017,7 @@
       <c r="Z221" s="9"/>
       <c r="AA221" s="9"/>
     </row>
-    <row r="222" spans="1:27" ht="28">
+    <row r="222" spans="1:27" ht="14">
       <c r="A222" s="9">
         <v>14</v>
       </c>
@@ -11017,7 +11028,7 @@
         <v>172</v>
       </c>
       <c r="D222" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E222" s="9"/>
       <c r="F222" s="9"/>
@@ -11043,7 +11054,7 @@
       <c r="Z222" s="9"/>
       <c r="AA222" s="9"/>
     </row>
-    <row r="223" spans="1:27" ht="14">
+    <row r="223" spans="1:27" ht="28">
       <c r="A223" s="9">
         <v>14</v>
       </c>
@@ -11054,7 +11065,7 @@
         <v>172</v>
       </c>
       <c r="D223" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E223" s="9"/>
       <c r="F223" s="9"/>
@@ -11091,7 +11102,7 @@
         <v>172</v>
       </c>
       <c r="D224" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E224" s="9"/>
       <c r="F224" s="9"/>
@@ -11127,8 +11138,8 @@
       <c r="C225" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D225" s="10" t="s">
-        <v>258</v>
+      <c r="D225" s="11" t="s">
+        <v>257</v>
       </c>
       <c r="E225" s="9"/>
       <c r="F225" s="9"/>
@@ -11154,7 +11165,7 @@
       <c r="Z225" s="9"/>
       <c r="AA225" s="9"/>
     </row>
-    <row r="226" spans="1:27" ht="28">
+    <row r="226" spans="1:27" ht="14">
       <c r="A226" s="9">
         <v>14</v>
       </c>
@@ -11164,8 +11175,8 @@
       <c r="C226" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D226" s="11" t="s">
-        <v>259</v>
+      <c r="D226" s="10" t="s">
+        <v>258</v>
       </c>
       <c r="E226" s="9"/>
       <c r="F226" s="9"/>
@@ -11191,7 +11202,7 @@
       <c r="Z226" s="9"/>
       <c r="AA226" s="9"/>
     </row>
-    <row r="227" spans="1:27" ht="14">
+    <row r="227" spans="1:27" ht="28">
       <c r="A227" s="9">
         <v>14</v>
       </c>
@@ -11201,8 +11212,8 @@
       <c r="C227" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D227" s="10" t="s">
-        <v>260</v>
+      <c r="D227" s="11" t="s">
+        <v>259</v>
       </c>
       <c r="E227" s="9"/>
       <c r="F227" s="9"/>
@@ -11239,7 +11250,7 @@
         <v>172</v>
       </c>
       <c r="D228" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E228" s="9"/>
       <c r="F228" s="9"/>
@@ -11275,8 +11286,8 @@
       <c r="C229" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D229" s="11" t="s">
-        <v>262</v>
+      <c r="D229" s="10" t="s">
+        <v>261</v>
       </c>
       <c r="E229" s="9"/>
       <c r="F229" s="9"/>
@@ -11312,8 +11323,8 @@
       <c r="C230" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D230" s="10" t="s">
-        <v>263</v>
+      <c r="D230" s="11" t="s">
+        <v>262</v>
       </c>
       <c r="E230" s="9"/>
       <c r="F230" s="9"/>
@@ -11350,7 +11361,7 @@
         <v>172</v>
       </c>
       <c r="D231" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E231" s="9"/>
       <c r="F231" s="9"/>
@@ -11376,11 +11387,19 @@
       <c r="Z231" s="9"/>
       <c r="AA231" s="9"/>
     </row>
-    <row r="232" spans="1:27">
-      <c r="A232" s="9"/>
-      <c r="B232" s="9"/>
-      <c r="C232" s="9"/>
-      <c r="D232" s="10"/>
+    <row r="232" spans="1:27" ht="14">
+      <c r="A232" s="9">
+        <v>14</v>
+      </c>
+      <c r="B232" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C232" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D232" s="10" t="s">
+        <v>264</v>
+      </c>
       <c r="E232" s="9"/>
       <c r="F232" s="9"/>
       <c r="G232" s="9"/>
@@ -33908,6 +33927,35 @@
       <c r="Y1008" s="9"/>
       <c r="Z1008" s="9"/>
       <c r="AA1008" s="9"/>
+    </row>
+    <row r="1009" spans="1:27">
+      <c r="A1009" s="9"/>
+      <c r="B1009" s="9"/>
+      <c r="C1009" s="9"/>
+      <c r="D1009" s="10"/>
+      <c r="E1009" s="9"/>
+      <c r="F1009" s="9"/>
+      <c r="G1009" s="9"/>
+      <c r="H1009" s="9"/>
+      <c r="I1009" s="9"/>
+      <c r="J1009" s="9"/>
+      <c r="K1009" s="9"/>
+      <c r="L1009" s="9"/>
+      <c r="M1009" s="9"/>
+      <c r="N1009" s="9"/>
+      <c r="O1009" s="9"/>
+      <c r="P1009" s="9"/>
+      <c r="Q1009" s="9"/>
+      <c r="R1009" s="9"/>
+      <c r="S1009" s="9"/>
+      <c r="T1009" s="9"/>
+      <c r="U1009" s="9"/>
+      <c r="V1009" s="9"/>
+      <c r="W1009" s="9"/>
+      <c r="X1009" s="9"/>
+      <c r="Y1009" s="9"/>
+      <c r="Z1009" s="9"/>
+      <c r="AA1009" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -33960,26 +34008,26 @@
     <hyperlink ref="D180" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
     <hyperlink ref="D181" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
     <hyperlink ref="D182" r:id="rId49" location="what-are-common-components" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="D191" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="D202" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="D205" r:id="rId52" location="getting-security-assurance-approvals-for-a-new-service" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="D207" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="D209" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="D211" r:id="rId55" location="architecture-documentation" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="D213" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="D214" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="D215" r:id="rId58" location="common-components" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
-    <hyperlink ref="D216" r:id="rId59" location="common-tooling" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
-    <hyperlink ref="D217" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
-    <hyperlink ref="D218" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="D219" r:id="rId62" location="architecture-documentation" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
-    <hyperlink ref="D220" r:id="rId63" location="content" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
-    <hyperlink ref="D221" r:id="rId64" location="design-to-maximise-uptime" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
-    <hyperlink ref="D222" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
-    <hyperlink ref="D223" r:id="rId66" location="continuous-delivery" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
-    <hyperlink ref="D224" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
-    <hyperlink ref="D226" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
-    <hyperlink ref="D229" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="D192" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="D203" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="D206" r:id="rId52" location="getting-security-assurance-approvals-for-a-new-service" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="D208" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="D210" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="D212" r:id="rId55" location="architecture-documentation" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="D214" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="D215" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="D216" r:id="rId58" location="common-components" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="D217" r:id="rId59" location="common-tooling" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="D218" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="D219" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="D220" r:id="rId62" location="architecture-documentation" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="D221" r:id="rId63" location="content" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="D222" r:id="rId64" location="design-to-maximise-uptime" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="D223" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="D224" r:id="rId66" location="continuous-delivery" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="D225" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="D227" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="D230" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>